<commit_message>
fix: ImageHuman and excel
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/ImageHuman.xlsx
+++ b/data/Spreadsheet_Data/ImageHuman.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085B1658-1FE2-FC4E-B145-7DF7B1A80AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72290D6-C179-174F-9F0F-9865E2FA8705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26780" yWindow="3580" windowWidth="39020" windowHeight="21360" xr2:uid="{7EED5AEB-F614-CE4A-AE23-7A550819DBDD}"/>
+    <workbookView xWindow="28540" yWindow="7620" windowWidth="39020" windowHeight="21360" xr2:uid="{7EED5AEB-F614-CE4A-AE23-7A550819DBDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,66 +40,12 @@
     <t>Bachmann-Gregor.jpeg</t>
   </si>
   <si>
-    <t>Balduin_ABrilliantPhoto_2022_15-1.jpeg</t>
-  </si>
-  <si>
-    <t>bw_cropped_Julien_ABrilliantPhoto_2023_17.jpeg</t>
-  </si>
-  <si>
-    <t>Christian_ABrilliantPhoto_2022_19.jpeg</t>
-  </si>
-  <si>
-    <t>Christina_ABrilliantPhoto_2022_09 (1).jpeg</t>
-  </si>
-  <si>
-    <t>DanielaM_ABrilliantPhoto_2022_06-1.jpeg</t>
-  </si>
-  <si>
-    <t>DanielaS_ABrilliantPhoto_2022_13-1_edite.jpeg</t>
-  </si>
-  <si>
-    <t>Dominique_ABrilliantPhoto_2022_06-1.jpeg</t>
-  </si>
-  <si>
-    <t>Flavie_ABrilliantPhoto_2022_06-1.jpeg</t>
-  </si>
-  <si>
-    <t>Irmantas_ABrilliantPhoto_2024_09bw.jpeg</t>
-  </si>
-  <si>
-    <t>Ivan_ABrilliantPhoto_2022_10-1 (1).jpeg</t>
-  </si>
-  <si>
-    <t>Johannes_ABrilliantPhoto_2022_03-1.jpeg</t>
-  </si>
-  <si>
-    <t>JoseLuis.jpeg</t>
-  </si>
-  <si>
-    <t>Julien_ABrilliantPhoto_2022_05-1 (1).jpeg</t>
-  </si>
-  <si>
-    <t>Lukas_ABrilliantPhoto_2022_04-1_edited_j.jpeg</t>
-  </si>
-  <si>
     <t>Marcin_ABrilliantPhoto_2022_14-1.jpeg</t>
   </si>
   <si>
-    <t>Noemi_November2022_12_.jpeg</t>
-  </si>
-  <si>
-    <t>nora.jpeg</t>
-  </si>
-  <si>
     <t>Raitis_ABrilliantPhoto_2024_09bw.jpeg</t>
   </si>
   <si>
-    <t>Rita_ABrilliantPhoto_2022_14-1 (1).jpeg</t>
-  </si>
-  <si>
-    <t>Samuel_ABrilliantPhoto_2022_07-1.jpeg</t>
-  </si>
-  <si>
     <t>IH_001</t>
   </si>
   <si>
@@ -254,6 +200,60 @@
   </si>
   <si>
     <t>Time Stamp</t>
+  </si>
+  <si>
+    <t>Julien_ABrilliantPhoto_2022_05.jpg</t>
+  </si>
+  <si>
+    <t>Samuel_ABrilliantPhoto_2022_07.jpg</t>
+  </si>
+  <si>
+    <t>Rita_ABrilliantPhoto_2022_14.jpg</t>
+  </si>
+  <si>
+    <t>Nora_ABrilliantPhoto_Feb2024_05.jpg</t>
+  </si>
+  <si>
+    <t>Noemi_November2022_12_.jpg</t>
+  </si>
+  <si>
+    <t>Lukas_ABrilliantPhoto_2022_04.jpg</t>
+  </si>
+  <si>
+    <t>Jose_ABrilliantPhoto_2024_04.jpg</t>
+  </si>
+  <si>
+    <t>Johannes_ABrilliantPhoto_2022_03.jpg</t>
+  </si>
+  <si>
+    <t>Ivan_ABrilliantPhoto_2022_10.jpg</t>
+  </si>
+  <si>
+    <t>Irmantas_ABrilliantPhoto_2024_09.jpg</t>
+  </si>
+  <si>
+    <t>Flavie_ABrilliantPhoto_2022_06.jpg</t>
+  </si>
+  <si>
+    <t>Dominique_ABrilliantPhoto_2022_06.jpg</t>
+  </si>
+  <si>
+    <t>DanielaS_ABrilliantPhoto_2022_13.jpg</t>
+  </si>
+  <si>
+    <t>DanielaM_ABrilliantPhoto_2022_06.jpg</t>
+  </si>
+  <si>
+    <t>Christina_ABrilliantPhoto_2022_09.jpg</t>
+  </si>
+  <si>
+    <t>Christian_ABrilliantPhoto_2022_19.jpg</t>
+  </si>
+  <si>
+    <t>Julien_ABrilliantPhoto_2023_17.jpg</t>
+  </si>
+  <si>
+    <t>Balduin_ABrilliantPhoto_2022_15.jpg</t>
   </si>
 </sst>
 </file>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63AE7FA7-C8FA-1B43-BF0F-01EE4860E752}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="221" zoomScaleNormal="221" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,445 +658,445 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
         <v>42</v>
-      </c>
-      <c r="E20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: add team image
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/ImageHuman.xlsx
+++ b/data/Spreadsheet_Data/ImageHuman.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEF1735-830B-FE4E-8694-604DD28E53A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C13CFD-D25E-7840-8ABD-0A4849DA5EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="500" windowWidth="64320" windowHeight="21360" xr2:uid="{7EED5AEB-F614-CE4A-AE23-7A550819DBDD}"/>
   </bookViews>
@@ -37,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
-    <t>Bachmann-Gregor.jpeg</t>
-  </si>
-  <si>
     <t>Marcin_ABrilliantPhoto_2022_14-1.jpeg</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>data/Multimedia_Data/Image_Human/</t>
+  </si>
+  <si>
+    <t>Gregor_ABrilliantPhoto_2022_04.jpg</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="221" zoomScaleNormal="221" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,442 +654,442 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>